<commit_message>
correções de bugs e modulo de acesso ao google sheets
</commit_message>
<xml_diff>
--- a/data/all_messages.xlsx
+++ b/data/all_messages.xlsx
@@ -464,17 +464,17 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>9:01 AM, 08/11/2023</t>
+          <t>6:16 PM, 08/11/2023</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Igor</t>
+          <t>toothbot</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>r</t>
+          <t>Placar Libertadores do Tooth</t>
         </is>
       </c>
     </row>
@@ -487,7 +487,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>9:01 AM, 08/11/2023</t>
+          <t>6:21 PM, 08/11/2023</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -497,7 +497,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>/placar</t>
         </is>
       </c>
     </row>
@@ -510,17 +510,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>9:01 AM, 08/11/2023</t>
+          <t>6:21 PM, 08/11/2023</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Igor</t>
+          <t>toothbot</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>Placar Libertadores do Tooth</t>
         </is>
       </c>
     </row>
@@ -533,7 +533,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0:46 PM, 08/11/2023</t>
+          <t>6:21 PM, 08/11/2023</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -543,7 +543,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Top Toother  |  No.Tooths</t>
         </is>
       </c>
     </row>
@@ -556,17 +556,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0:50 PM, 08/11/2023</t>
+          <t>6:21 PM, 08/11/2023</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Igor</t>
+          <t>toothbot</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>/placar</t>
+          <t>1.   Igor    3</t>
         </is>
       </c>
     </row>
@@ -579,7 +579,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>4:53 PM, 08/11/2023</t>
+          <t>6:23 PM, 08/11/2023</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -602,12 +602,12 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>5:09 PM, 08/11/2023</t>
+          <t>9:26 PM, 08/11/2023</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Igor</t>
+          <t>toothbot</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -625,17 +625,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>5:21 PM, 08/11/2023</t>
+          <t>9:28 PM, 08/11/2023</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>toothbot</t>
+          <t>Igor</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Toother</t>
+          <t>/placar</t>
         </is>
       </c>
     </row>
@@ -648,7 +648,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>5:29 PM, 08/11/2023</t>
+          <t>9:28 PM, 08/11/2023</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -658,7 +658,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>/placar</t>
+          <t>💩</t>
         </is>
       </c>
     </row>
@@ -671,17 +671,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>5:33 PM, 08/11/2023</t>
+          <t>9:28 PM, 08/11/2023</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>toothbot</t>
+          <t>Igor</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Igor    3Toother</t>
+          <t>/placar</t>
         </is>
       </c>
     </row>
@@ -694,17 +694,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>5:35 PM, 08/11/2023</t>
+          <t>8:22 AM, 09/11/2023</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Igor</t>
+          <t>toothbot</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>/placar</t>
+          <t>Placar Libertadores do Tooth</t>
         </is>
       </c>
     </row>
@@ -717,7 +717,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>5:35 PM, 08/11/2023</t>
+          <t>8:22 AM, 09/11/2023</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -727,7 +727,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Igor    3T o o t h e r</t>
+          <t>Top Toother  |  No.Tooths</t>
         </is>
       </c>
     </row>
@@ -740,7 +740,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>5:41 PM, 08/11/2023</t>
+          <t>8:22 AM, 09/11/2023</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -750,7 +750,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>/placar</t>
+          <t>1.   Igor           1</t>
         </is>
       </c>
     </row>
@@ -763,17 +763,17 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>6:01 PM, 08/11/2023</t>
+          <t>8:23 AM, 09/11/2023</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>toothbot</t>
+          <t>Igor</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Placar Libertadores do Tooth</t>
+          <t>💩</t>
         </is>
       </c>
     </row>
@@ -786,17 +786,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>6:01 PM, 08/11/2023</t>
+          <t>8:24 AM, 09/11/2023</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>toothbot</t>
+          <t>Igor</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Top Toother  |  No.Tooths</t>
+          <t>/placar</t>
         </is>
       </c>
     </row>
@@ -809,7 +809,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>6:01 PM, 08/11/2023</t>
+          <t>8:24 AM, 09/11/2023</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -819,7 +819,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1.   Igor    18</t>
+          <t>Placar Libertadores do Tooth</t>
         </is>
       </c>
     </row>
@@ -832,7 +832,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>6:03 PM, 08/11/2023</t>
+          <t>8:24 AM, 09/11/2023</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -842,7 +842,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>/placar</t>
+          <t>Top Toother  |  No.Tooths</t>
         </is>
       </c>
     </row>
@@ -855,7 +855,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>6:07 PM, 08/11/2023</t>
+          <t>8:24 AM, 09/11/2023</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -865,7 +865,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Placar Libertadores do Tooth</t>
+          <t>1.   Igor           2</t>
         </is>
       </c>
     </row>
@@ -878,12 +878,12 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>6:10 PM, 08/11/2023</t>
+          <t>8:27 AM, 09/11/2023</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>toothbot</t>
+          <t>Igor</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -901,7 +901,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>6:10 PM, 08/11/2023</t>
+          <t>8:28 AM, 09/11/2023</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -924,7 +924,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>6:12 PM, 08/11/2023</t>
+          <t>8:28 AM, 09/11/2023</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -934,7 +934,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>/placar</t>
+          <t>Top Toother  |  No.Tooths</t>
         </is>
       </c>
     </row>
@@ -947,7 +947,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>6:14 PM, 08/11/2023</t>
+          <t>8:28 AM, 09/11/2023</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -957,7 +957,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Placar Libertadores do Tooth</t>
+          <t>1.   Igor           5</t>
         </is>
       </c>
     </row>
@@ -966,11 +966,11 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>6:16 PM, 08/11/2023</t>
+          <t>5:27 PM, 09/11/2023</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -989,21 +989,21 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>6:16 PM, 08/11/2023</t>
+          <t>10:44 PM, 09/11/2023</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>toothbot</t>
+          <t>Igor</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Placar Libertadores do Tooth</t>
+          <t>/placar</t>
         </is>
       </c>
     </row>
@@ -1012,21 +1012,21 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>6:21 PM, 08/11/2023</t>
+          <t>10:56 PM, 09/11/2023</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Igor</t>
+          <t>toothbot</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>/placar</t>
+          <t>[</t>
         </is>
       </c>
     </row>
@@ -1035,11 +1035,11 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>6:21 PM, 08/11/2023</t>
+          <t>10:56 PM, 09/11/2023</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1049,7 +1049,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Placar Libertadores do Tooth</t>
+          <t>{</t>
         </is>
       </c>
     </row>
@@ -1058,11 +1058,11 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>6:21 PM, 08/11/2023</t>
+          <t>10:56 PM, 09/11/2023</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1072,7 +1072,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Top Toother  |  No.Tooths</t>
+          <t>'</t>
         </is>
       </c>
     </row>
@@ -1081,11 +1081,11 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>6:21 PM, 08/11/2023</t>
+          <t>10:56 PM, 09/11/2023</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1095,7 +1095,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>1.   Igor    3</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -1104,21 +1104,21 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>6:23 PM, 08/11/2023</t>
+          <t>10:56 PM, 09/11/2023</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Igor</t>
+          <t>toothbot</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>/placar</t>
+          <t>9</t>
         </is>
       </c>
     </row>
@@ -1127,11 +1127,11 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>9:26 PM, 08/11/2023</t>
+          <t>10:56 PM, 09/11/2023</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1141,7 +1141,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>/placar</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -1150,21 +1150,21 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>9:28 PM, 08/11/2023</t>
+          <t>10:56 PM, 09/11/2023</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Igor</t>
+          <t>toothbot</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>/placar</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -1173,21 +1173,21 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>9:28 PM, 08/11/2023</t>
+          <t>10:56 PM, 09/11/2023</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Igor</t>
+          <t>toothbot</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>💩</t>
+          <t>'</t>
         </is>
       </c>
     </row>
@@ -1196,21 +1196,21 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>9:28 PM, 08/11/2023</t>
+          <t>10:56 PM, 09/11/2023</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Igor</t>
+          <t>toothbot</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>/placar</t>
+          <t>:</t>
         </is>
       </c>
     </row>
@@ -1219,11 +1219,11 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>8:22 AM, 09/11/2023</t>
+          <t>10:56 PM, 09/11/2023</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1233,7 +1233,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Placar Libertadores do Tooth</t>
+          <t>[</t>
         </is>
       </c>
     </row>
@@ -1242,11 +1242,11 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>8:22 AM, 09/11/2023</t>
+          <t>10:56 PM, 09/11/2023</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1256,7 +1256,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Top Toother  |  No.Tooths</t>
+          <t>{</t>
         </is>
       </c>
     </row>
@@ -1265,11 +1265,11 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>8:22 AM, 09/11/2023</t>
+          <t>10:56 PM, 09/11/2023</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1279,7 +1279,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>1.   Igor           1</t>
+          <t>'</t>
         </is>
       </c>
     </row>
@@ -1288,21 +1288,21 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>8:23 AM, 09/11/2023</t>
+          <t>10:56 PM, 09/11/2023</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Igor</t>
+          <t>toothbot</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>💩</t>
+          <t>I</t>
         </is>
       </c>
     </row>
@@ -1311,21 +1311,21 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>8:24 AM, 09/11/2023</t>
+          <t>10:56 PM, 09/11/2023</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Igor</t>
+          <t>toothbot</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>/placar</t>
+          <t>g</t>
         </is>
       </c>
     </row>
@@ -1334,11 +1334,11 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>8:24 AM, 09/11/2023</t>
+          <t>10:56 PM, 09/11/2023</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1348,7 +1348,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Placar Libertadores do Tooth</t>
+          <t>o</t>
         </is>
       </c>
     </row>
@@ -1357,11 +1357,11 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>8:24 AM, 09/11/2023</t>
+          <t>10:56 PM, 09/11/2023</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1371,7 +1371,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Top Toother  |  No.Tooths</t>
+          <t>r</t>
         </is>
       </c>
     </row>
@@ -1380,11 +1380,11 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>8:24 AM, 09/11/2023</t>
+          <t>10:56 PM, 09/11/2023</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -1394,7 +1394,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>1.   Igor           2</t>
+          <t>'</t>
         </is>
       </c>
     </row>
@@ -1403,21 +1403,21 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>8:27 AM, 09/11/2023</t>
+          <t>10:56 PM, 09/11/2023</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Igor</t>
+          <t>toothbot</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>/placar</t>
+          <t>:</t>
         </is>
       </c>
     </row>
@@ -1426,11 +1426,11 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>8:28 AM, 09/11/2023</t>
+          <t>10:56 PM, 09/11/2023</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -1440,7 +1440,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Placar Libertadores do Tooth</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -1449,11 +1449,11 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>8:28 AM, 09/11/2023</t>
+          <t>10:57 PM, 09/11/2023</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -1463,7 +1463,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Top Toother  |  No.Tooths</t>
+          <t>}</t>
         </is>
       </c>
     </row>
@@ -1472,11 +1472,11 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>8:28 AM, 09/11/2023</t>
+          <t>10:57 PM, 09/11/2023</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1486,7 +1486,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>1.   Igor           5</t>
+          <t>]</t>
         </is>
       </c>
     </row>
@@ -1499,17 +1499,17 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>5:27 PM, 09/11/2023</t>
+          <t>10:57 PM, 09/11/2023</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Igor</t>
+          <t>toothbot</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>/placar</t>
+          <t>}</t>
         </is>
       </c>
     </row>
@@ -1522,17 +1522,17 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>10:44 PM, 09/11/2023</t>
+          <t>10:57 PM, 09/11/2023</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Igor</t>
+          <t>toothbot</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>/placar</t>
+          <t>]</t>
         </is>
       </c>
     </row>

</xml_diff>